<commit_message>
modified in seed data
</commit_message>
<xml_diff>
--- a/service-provider-profile-service/src/main/resources/sp-profile-service.xlsx
+++ b/service-provider-profile-service/src/main/resources/sp-profile-service.xlsx
@@ -2740,12 +2740,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2761,6 +2760,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2843,7 +2848,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2853,31 +2858,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2901,25 +2906,24 @@
   </sheetPr>
   <dimension ref="A1:M256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -3456,7 +3460,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
@@ -4727,7 +4731,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>231</v>
       </c>
@@ -4768,7 +4772,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
         <v>234</v>
       </c>
@@ -4809,7 +4813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>238</v>
       </c>
@@ -4850,7 +4854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
         <v>241</v>
       </c>
@@ -4891,7 +4895,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
         <v>244</v>
       </c>
@@ -4932,7 +4936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
         <v>247</v>
       </c>
@@ -4973,7 +4977,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
         <v>250</v>
       </c>
@@ -5014,7 +5018,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
         <v>253</v>
       </c>
@@ -5055,7 +5059,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
         <v>256</v>
       </c>
@@ -5096,7 +5100,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>259</v>
       </c>
@@ -5137,7 +5141,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>262</v>
       </c>
@@ -5178,7 +5182,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>266</v>
       </c>
@@ -5219,7 +5223,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
         <v>269</v>
       </c>
@@ -5260,7 +5264,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
         <v>272</v>
       </c>
@@ -5301,7 +5305,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
         <v>275</v>
       </c>
@@ -5342,7 +5346,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
         <v>278</v>
       </c>
@@ -5383,7 +5387,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
         <v>281</v>
       </c>
@@ -5424,7 +5428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
         <v>284</v>
       </c>
@@ -5465,7 +5469,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>287</v>
       </c>
@@ -5506,7 +5510,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>290</v>
       </c>
@@ -5547,7 +5551,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>294</v>
       </c>
@@ -5998,7 +6002,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>330</v>
       </c>
@@ -6039,7 +6043,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>333</v>
       </c>
@@ -6080,7 +6084,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
         <v>336</v>
       </c>
@@ -6121,7 +6125,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
         <v>339</v>
       </c>
@@ -6162,7 +6166,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
         <v>341</v>
       </c>
@@ -6203,7 +6207,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
         <v>344</v>
       </c>
@@ -6244,7 +6248,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>347</v>
       </c>
@@ -6285,7 +6289,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
         <v>350</v>
       </c>
@@ -6326,7 +6330,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
         <v>354</v>
       </c>
@@ -6367,7 +6371,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
         <v>357</v>
       </c>
@@ -6408,7 +6412,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
         <v>360</v>
       </c>
@@ -6449,7 +6453,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
         <v>363</v>
       </c>
@@ -6490,7 +6494,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
         <v>366</v>
       </c>
@@ -6531,7 +6535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
         <v>369</v>
       </c>
@@ -6572,7 +6576,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
         <v>372</v>
       </c>
@@ -6613,7 +6617,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
         <v>375</v>
       </c>
@@ -6654,7 +6658,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
         <v>378</v>
       </c>
@@ -6695,7 +6699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
         <v>382</v>
       </c>
@@ -6736,7 +6740,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
         <v>385</v>
       </c>
@@ -6777,7 +6781,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
         <v>388</v>
       </c>
@@ -6818,7 +6822,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
         <v>391</v>
       </c>
@@ -6859,7 +6863,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
         <v>394</v>
       </c>
@@ -6900,7 +6904,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
         <v>397</v>
       </c>
@@ -6941,7 +6945,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
         <v>400</v>
       </c>
@@ -6982,7 +6986,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
         <v>403</v>
       </c>
@@ -7023,7 +7027,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
         <v>406</v>
       </c>
@@ -7064,7 +7068,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
         <v>410</v>
       </c>
@@ -7105,7 +7109,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
         <v>413</v>
       </c>
@@ -7146,7 +7150,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
         <v>416</v>
       </c>
@@ -7187,7 +7191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
         <v>419</v>
       </c>
@@ -7228,7 +7232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
         <v>422</v>
       </c>
@@ -7269,7 +7273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
         <v>425</v>
       </c>
@@ -7310,7 +7314,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
         <v>428</v>
       </c>
@@ -7351,7 +7355,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
         <v>431</v>
       </c>
@@ -7392,7 +7396,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
         <v>434</v>
       </c>
@@ -7433,7 +7437,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
         <v>437</v>
       </c>
@@ -7474,7 +7478,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
         <v>440</v>
       </c>
@@ -7515,7 +7519,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
         <v>444</v>
       </c>
@@ -7556,7 +7560,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
         <v>447</v>
       </c>
@@ -7597,7 +7601,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
         <v>450</v>
       </c>
@@ -7638,7 +7642,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
         <v>453</v>
       </c>
@@ -7679,7 +7683,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
         <v>456</v>
       </c>
@@ -7720,7 +7724,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
         <v>459</v>
       </c>
@@ -7761,7 +7765,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
         <v>462</v>
       </c>
@@ -7802,7 +7806,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
         <v>465</v>
       </c>
@@ -7843,7 +7847,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
         <v>468</v>
       </c>
@@ -7884,7 +7888,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
         <v>472</v>
       </c>
@@ -7925,7 +7929,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
         <v>475</v>
       </c>
@@ -7966,7 +7970,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
         <v>478</v>
       </c>
@@ -8007,7 +8011,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
         <v>481</v>
       </c>
@@ -8048,7 +8052,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
         <v>484</v>
       </c>
@@ -8089,7 +8093,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
         <v>487</v>
       </c>
@@ -8130,7 +8134,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
         <v>490</v>
       </c>
@@ -8171,7 +8175,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
         <v>493</v>
       </c>
@@ -8212,7 +8216,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
         <v>496</v>
       </c>
@@ -8253,7 +8257,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
         <v>500</v>
       </c>
@@ -8294,7 +8298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
         <v>503</v>
       </c>
@@ -8335,7 +8339,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
         <v>506</v>
       </c>
@@ -8376,7 +8380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
         <v>509</v>
       </c>
@@ -8417,7 +8421,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
         <v>512</v>
       </c>
@@ -8458,7 +8462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
         <v>515</v>
       </c>
@@ -8499,7 +8503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
         <v>518</v>
       </c>
@@ -8540,7 +8544,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
         <v>521</v>
       </c>
@@ -8581,7 +8585,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
         <v>524</v>
       </c>
@@ -8622,7 +8626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
         <v>527</v>
       </c>
@@ -8663,7 +8667,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
         <v>531</v>
       </c>
@@ -8704,7 +8708,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
         <v>534</v>
       </c>
@@ -8745,7 +8749,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
         <v>537</v>
       </c>
@@ -8786,7 +8790,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="s">
         <v>540</v>
       </c>
@@ -8827,7 +8831,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="5" t="s">
         <v>543</v>
       </c>
@@ -8868,7 +8872,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
         <v>546</v>
       </c>
@@ -8909,7 +8913,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
         <v>549</v>
       </c>
@@ -8950,7 +8954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
         <v>552</v>
       </c>
@@ -8991,7 +8995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
         <v>556</v>
       </c>
@@ -9032,7 +9036,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
         <v>559</v>
       </c>
@@ -9073,7 +9077,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="5" t="s">
         <v>562</v>
       </c>
@@ -9114,7 +9118,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
         <v>565</v>
       </c>
@@ -9155,7 +9159,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="5" t="s">
         <v>568</v>
       </c>
@@ -9196,7 +9200,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
         <v>571</v>
       </c>
@@ -9237,7 +9241,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="5" t="s">
         <v>574</v>
       </c>
@@ -9278,7 +9282,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
         <v>577</v>
       </c>
@@ -9319,7 +9323,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="5" t="s">
         <v>581</v>
       </c>
@@ -9360,7 +9364,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="5" t="s">
         <v>584</v>
       </c>
@@ -9401,7 +9405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="5" t="s">
         <v>587</v>
       </c>
@@ -9442,7 +9446,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="5" t="s">
         <v>590</v>
       </c>
@@ -9483,7 +9487,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="5" t="s">
         <v>593</v>
       </c>
@@ -9524,7 +9528,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="5" t="s">
         <v>596</v>
       </c>
@@ -9565,7 +9569,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="5" t="s">
         <v>599</v>
       </c>
@@ -9606,7 +9610,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="5" t="s">
         <v>602</v>
       </c>
@@ -9647,7 +9651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="5" t="s">
         <v>606</v>
       </c>
@@ -9688,7 +9692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="5" t="s">
         <v>609</v>
       </c>
@@ -9729,7 +9733,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="5" t="s">
         <v>612</v>
       </c>
@@ -9770,7 +9774,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="5" t="s">
         <v>615</v>
       </c>
@@ -9811,7 +9815,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="5" t="s">
         <v>617</v>
       </c>
@@ -9852,7 +9856,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="5" t="s">
         <v>620</v>
       </c>
@@ -9893,7 +9897,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="5" t="s">
         <v>623</v>
       </c>
@@ -9934,7 +9938,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="5" t="s">
         <v>626</v>
       </c>
@@ -9975,7 +9979,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="5" t="s">
         <v>630</v>
       </c>
@@ -10016,7 +10020,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
         <v>633</v>
       </c>
@@ -10057,7 +10061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="5" t="s">
         <v>636</v>
       </c>
@@ -10098,7 +10102,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
         <v>639</v>
       </c>
@@ -10139,7 +10143,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="5" t="s">
         <v>642</v>
       </c>
@@ -10180,7 +10184,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
         <v>645</v>
       </c>
@@ -10221,7 +10225,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="5" t="s">
         <v>648</v>
       </c>
@@ -10262,7 +10266,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="5" t="s">
         <v>651</v>
       </c>
@@ -10303,7 +10307,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="5" t="s">
         <v>654</v>
       </c>
@@ -10344,7 +10348,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
         <v>657</v>
       </c>
@@ -10385,7 +10389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="5" t="s">
         <v>661</v>
       </c>
@@ -10426,7 +10430,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="5" t="s">
         <v>664</v>
       </c>
@@ -10467,7 +10471,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="5" t="s">
         <v>667</v>
       </c>
@@ -10508,7 +10512,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
         <v>670</v>
       </c>
@@ -10549,7 +10553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="5" t="s">
         <v>673</v>
       </c>
@@ -10590,7 +10594,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
         <v>676</v>
       </c>
@@ -10631,7 +10635,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="5" t="s">
         <v>679</v>
       </c>
@@ -10672,7 +10676,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="5" t="s">
         <v>682</v>
       </c>
@@ -10713,7 +10717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="5" t="s">
         <v>686</v>
       </c>
@@ -10754,7 +10758,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="5" t="s">
         <v>689</v>
       </c>
@@ -10795,7 +10799,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="5" t="s">
         <v>692</v>
       </c>
@@ -10836,7 +10840,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="5" t="s">
         <v>695</v>
       </c>
@@ -10877,7 +10881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="5" t="s">
         <v>698</v>
       </c>
@@ -10918,7 +10922,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="5" t="s">
         <v>701</v>
       </c>
@@ -10959,7 +10963,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="5" t="s">
         <v>704</v>
       </c>
@@ -11000,7 +11004,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
         <v>708</v>
       </c>
@@ -11041,7 +11045,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="5" t="s">
         <v>711</v>
       </c>
@@ -11082,7 +11086,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="5" t="s">
         <v>714</v>
       </c>
@@ -11123,7 +11127,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="5" t="s">
         <v>717</v>
       </c>
@@ -11164,7 +11168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="5" t="s">
         <v>720</v>
       </c>
@@ -11205,7 +11209,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="5" t="s">
         <v>723</v>
       </c>
@@ -11246,7 +11250,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="5" t="s">
         <v>726</v>
       </c>
@@ -11287,7 +11291,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="5" t="s">
         <v>729</v>
       </c>
@@ -11328,7 +11332,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="5" t="s">
         <v>732</v>
       </c>
@@ -11369,7 +11373,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="5" t="s">
         <v>736</v>
       </c>
@@ -11410,7 +11414,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="5" t="s">
         <v>739</v>
       </c>
@@ -11451,7 +11455,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="5" t="s">
         <v>742</v>
       </c>
@@ -11492,7 +11496,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="5" t="s">
         <v>745</v>
       </c>
@@ -11533,7 +11537,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="5" t="s">
         <v>748</v>
       </c>
@@ -11574,7 +11578,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="5" t="s">
         <v>751</v>
       </c>
@@ -11615,7 +11619,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="5" t="s">
         <v>754</v>
       </c>
@@ -11656,7 +11660,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="5" t="s">
         <v>757</v>
       </c>
@@ -11697,7 +11701,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="5" t="s">
         <v>761</v>
       </c>
@@ -11738,7 +11742,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="5" t="s">
         <v>764</v>
       </c>
@@ -11779,7 +11783,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="5" t="s">
         <v>602</v>
       </c>
@@ -11820,7 +11824,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="5" t="s">
         <v>768</v>
       </c>
@@ -11861,7 +11865,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="5" t="s">
         <v>771</v>
       </c>
@@ -11902,7 +11906,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="5" t="s">
         <v>774</v>
       </c>
@@ -11943,7 +11947,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="5" t="s">
         <v>777</v>
       </c>
@@ -12312,7 +12316,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="5" t="s">
         <v>810</v>
       </c>

</xml_diff>